<commit_message>
modified:   fixture_list.xlsx 	modified:   services_portal_metrics.py
</commit_message>
<xml_diff>
--- a/fixture_list.xlsx
+++ b/fixture_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78BC5C7-537F-6643-8DE8-5FE70CFA58B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DA82A9-BE6C-CD4F-A217-E78CB0B169D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2900" windowWidth="26440" windowHeight="14120" xr2:uid="{6210E12D-6C9B-F840-A533-7641B31E3720}"/>
+    <workbookView xWindow="71920" yWindow="1280" windowWidth="30240" windowHeight="19020" xr2:uid="{6210E12D-6C9B-F840-A533-7641B31E3720}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>Fixture Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Robbie Williams Live 2025 - Saturday</t>
   </si>
@@ -165,12 +162,21 @@
   </si>
   <si>
     <t>Arsenal v Bayer 04 Leverkusen</t>
+  </si>
+  <si>
+    <t>FixtureName</t>
+  </si>
+  <si>
+    <t>EventDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -181,7 +187,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -208,9 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,230 +552,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC35374-5C33-C541-9FD8-223C780A5849}">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="2">
+        <v>45815.6875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" s="2">
+        <v>45814.6875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="2">
+        <v>45795.583333333343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" s="2">
+        <v>45787.479166666657</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" s="2">
+        <v>45780.6875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" s="2">
+        <v>45773.6875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" s="2">
+        <v>45759.6875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="2">
+        <v>45755.791666666657</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" s="2">
+        <v>45748.78125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="2">
+        <v>45742.833333333343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="2">
+        <v>45738.729166666657</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" s="2">
+        <v>45732.5625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" s="2">
+        <v>45728.833333333343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" s="2">
+        <v>45710.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" s="2">
+        <v>45704.520833333343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" s="2">
+        <v>45690.6875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" s="2">
+        <v>45679.833333333343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" s="2">
+        <v>45675.729166666657</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20" s="2">
+        <v>45672.833333333343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" s="2">
+        <v>45669.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45664.833333333343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B23" s="2">
+        <v>45653.84375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45644.8125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B25" s="2">
+        <v>45644.833333333343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B26" s="2">
+        <v>45640.625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B27" s="2">
+        <v>45637.833333333343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B28" s="2">
+        <v>45634.583333333343</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45630.84375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B30" s="2">
+        <v>45619.625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B31" s="2">
+        <v>45617.833333333343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B32" s="2">
+        <v>45604.791666666657</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B33" s="2">
+        <v>45592.6875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B34" s="2">
+        <v>45587.791666666657</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B35" s="2">
+        <v>45581.791666666657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B36" s="2">
+        <v>45577.53125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B37" s="2">
+        <v>45571.541666666657</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B38" s="2">
+        <v>45570.583333333343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B39" s="2">
+        <v>45566.791666666657</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B40" s="2">
+        <v>45563.583333333343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B41" s="2">
+        <v>45560.78125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B42" s="2">
+        <v>45557.479166666657</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B43" s="2">
+        <v>45535.479166666657</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B44" s="2">
+        <v>45521.583333333343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B45" s="2">
+        <v>45515.541666666657</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>42</v>
+      <c r="B46" s="2">
+        <v>45511.708333333343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>